<commit_message>
Yield table testing framework
</commit_message>
<xml_diff>
--- a/backend/src/test/java/ca/bc/gov/nrs/vdyp/backend/endpoints/projection/hcsv/scenarios/scenarios.xlsx
+++ b/backend/src/test/java/ca/bc/gov/nrs/vdyp/backend/endpoints/projection/hcsv/scenarios/scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjunkin/source/vdyp-ssh/backend/src/test/java/ca/bc/gov/nrs/vdyp/backend/endpoints/projection/hcsv/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B7F4DB-BDF2-8D4A-B349-D18335921694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0EA717-727F-8948-87AB-2ED6AD493712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{B61BCA9A-1318-5A42-A1CB-31D8A51730BF}"/>
   </bookViews>
@@ -36,34 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Output File</t>
-  </si>
-  <si>
-    <t>Scenario1</t>
-  </si>
-  <si>
-    <t>Scenario2</t>
-  </si>
-  <si>
-    <t>Scenario3</t>
-  </si>
-  <si>
-    <t>Input Polygon File</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input Layer File </t>
-  </si>
-  <si>
-    <t>VDYP7_INPUT_POLY_VRI.csv</t>
-  </si>
-  <si>
-    <t>VDYP7_INPUT_LAYER_VRI.csv</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>Debug Log?</t>
   </si>
@@ -86,16 +59,37 @@
     <t>Include MoF Volumes?</t>
   </si>
   <si>
-    <t>VDYP7_INPUT_POLY_FIP.csv</t>
-  </si>
-  <si>
-    <t>VDYP7_INPUT_LAYER_FIP.csv</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>Include Projections</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Successful VRI run, one poly, one layer</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Successful FIP run, one poly, one layer</t>
+  </si>
+  <si>
+    <t>Text yield table generation verification. Plus, a number of tests of various start/end ages and start/end years.</t>
+  </si>
+  <si>
+    <t>Tests various combinations of start/end ages and start/end years.</t>
+  </si>
+  <si>
+    <t>Successful VRI run, one ploy, three layers. Only dead layer is projected because age params require only backwards projection for the non-dead layers</t>
+  </si>
+  <si>
+    <t>Tests parameters that add columns and specific rows to yield tables</t>
+  </si>
+  <si>
+    <t>Tests parameters that disable year and age rows being presented in yield tables</t>
   </si>
 </sst>
 </file>
@@ -483,154 +477,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F773A25-92B9-924E-A268-0C20AC65EEB1}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="3"/>
-    <col min="7" max="7" width="12.5" style="3" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="3"/>
-    <col min="10" max="10" width="10.83203125" style="2"/>
-    <col min="11" max="11" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="9.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="71.1640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="12.5" style="3" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B10" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>